<commit_message>
Update argparse descriptions and move old scripts to folder.
</commit_message>
<xml_diff>
--- a/results/vel-rms-slopes.xlsx
+++ b/results/vel-rms-slopes.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matro\Documents\AIUC\PythonScripts\CamCalib\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE6CD2B8-0BA1-45C0-89B2-7803B5B94FBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB99F176-091D-4D92-A72D-B2F63505CD30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Slopes" sheetId="1" r:id="rId1"/>
+    <sheet name="Calibration parameters" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Test</t>
   </si>
@@ -73,6 +74,42 @@
   </si>
   <si>
     <t>Wg. Aver.</t>
+  </si>
+  <si>
+    <t>fx</t>
+  </si>
+  <si>
+    <t>fy</t>
+  </si>
+  <si>
+    <t>cx</t>
+  </si>
+  <si>
+    <t>cy</t>
+  </si>
+  <si>
+    <t>k1</t>
+  </si>
+  <si>
+    <t>k2</t>
+  </si>
+  <si>
+    <t>p1</t>
+  </si>
+  <si>
+    <t>p2</t>
+  </si>
+  <si>
+    <t>k3</t>
+  </si>
+  <si>
+    <t>mean (mu)</t>
+  </si>
+  <si>
+    <t>error (sigma)</t>
+  </si>
+  <si>
+    <t>sigma/mean</t>
   </si>
 </sst>
 </file>
@@ -104,7 +141,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -215,11 +252,77 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -253,6 +356,22 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -534,185 +653,352 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:G11"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="5" width="18.33203125" customWidth="1"/>
-    <col min="6" max="6" width="19.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="18.33203125" customWidth="1"/>
+    <col min="5" max="5" width="19.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B2" s="12" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="B1" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="C1" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="D1" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="17" t="s">
+      <c r="E1" s="17" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B3" s="10" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="10" t="s">
         <v>1</v>
       </c>
+      <c r="B2" s="8">
+        <v>4.1515545600000001</v>
+      </c>
+      <c r="C2" s="8">
+        <v>1.46567775</v>
+      </c>
+      <c r="D2" s="8">
+        <v>0.754254399500074</v>
+      </c>
+      <c r="E2" s="1">
+        <f>D2/SUM($D$2:$D$6)</f>
+        <v>0.25390687612274054</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="8">
+        <v>3.5757802000000001</v>
+      </c>
       <c r="C3" s="8">
-        <v>4.1515545600000001</v>
+        <v>3.3244167400000002</v>
       </c>
       <c r="D3" s="8">
-        <v>1.46567775</v>
-      </c>
-      <c r="E3" s="8">
-        <v>0.754254399500074</v>
-      </c>
-      <c r="F3" s="1">
-        <f>E3/SUM($E$3:$E$7)</f>
-        <v>0.25390687612274054</v>
-      </c>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B4" s="10" t="s">
-        <v>2</v>
+        <v>0.55560664285158001</v>
+      </c>
+      <c r="E3" s="1">
+        <f t="shared" ref="E3:E6" si="0">D3/SUM($D$2:$D$6)</f>
+        <v>0.1870354977484941</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="8">
+        <v>3.42446538</v>
       </c>
       <c r="C4" s="8">
-        <v>3.5757802000000001</v>
+        <v>2.4944842199999999</v>
       </c>
       <c r="D4" s="8">
-        <v>3.3244167400000002</v>
-      </c>
-      <c r="E4" s="8">
-        <v>0.55560664285158001</v>
-      </c>
-      <c r="F4" s="1">
-        <f t="shared" ref="F4:F7" si="0">E4/SUM($E$3:$E$7)</f>
-        <v>0.1870354977484941</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B5" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="8">
-        <v>3.42446538</v>
-      </c>
-      <c r="D5" s="8">
-        <v>2.4944842199999999</v>
-      </c>
-      <c r="E5" s="8">
         <v>0.60459679853702097</v>
       </c>
-      <c r="F5" s="1">
+      <c r="E4" s="1">
         <f t="shared" si="0"/>
         <v>0.20352719789515769</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B6" s="10" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="8">
+      <c r="B5" s="8">
         <v>3.5528141999999998</v>
       </c>
-      <c r="D6" s="8">
+      <c r="C5" s="8">
         <v>1.36033424</v>
       </c>
-      <c r="E6" s="8">
+      <c r="D5" s="8">
         <v>0.73815665935675401</v>
       </c>
-      <c r="F6" s="1">
+      <c r="E5" s="1">
         <f t="shared" si="0"/>
         <v>0.24848784652856762</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B7" s="11" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="9">
+      <c r="B6" s="9">
         <v>2.1283324399999999</v>
       </c>
-      <c r="D7" s="9">
+      <c r="C6" s="9">
         <v>8.4959078100000003</v>
       </c>
-      <c r="E7" s="9">
+      <c r="D6" s="9">
         <v>0.31798011703252799</v>
       </c>
-      <c r="F7" s="6">
+      <c r="E6" s="6">
         <f t="shared" si="0"/>
         <v>0.10704258170504008</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B8" s="13" t="s">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="5">
-        <f>AVERAGE(C3:C7)</f>
+      <c r="B7" s="5">
+        <f>AVERAGE(B2:B6)</f>
         <v>3.366589356</v>
       </c>
-      <c r="D8" s="5">
-        <f t="shared" ref="D8:E8" si="1">AVERAGE(D3:D7)</f>
+      <c r="C7" s="5">
+        <f t="shared" ref="C7:D7" si="1">AVERAGE(C2:C6)</f>
         <v>3.4281641519999999</v>
       </c>
-      <c r="E8" s="7">
+      <c r="D7" s="7">
         <f t="shared" si="1"/>
         <v>0.59411892345559136</v>
       </c>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B9" s="13" t="s">
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="5">
-        <f>_xlfn.STDEV.S(C3:C7)</f>
+      <c r="B8" s="5">
+        <f>_xlfn.STDEV.S(B2:B6)</f>
         <v>0.74686690537921419</v>
       </c>
-      <c r="D9" s="5">
-        <f t="shared" ref="D9:E9" si="2">_xlfn.STDEV.S(D3:D7)</f>
+      <c r="C8" s="5">
+        <f t="shared" ref="C8:D8" si="2">_xlfn.STDEV.S(C2:C6)</f>
         <v>2.9449881556261084</v>
       </c>
-      <c r="E9" s="1">
+      <c r="D8" s="1">
         <f t="shared" si="2"/>
         <v>0.17623553989464252</v>
       </c>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B10" s="14" t="s">
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="3">
-        <f>SUMPRODUCT(C3:C7,$F$3:$F$7)</f>
+      <c r="B9" s="3">
+        <f>SUMPRODUCT(B2:B6,$E$2:$E$6)</f>
         <v>3.5305312707876078</v>
       </c>
-      <c r="D10" s="3">
-        <f t="shared" ref="D10:E10" si="3">SUMPRODUCT(D3:D7,$F$3:$F$7)</f>
+      <c r="C9" s="3">
+        <f t="shared" ref="C9:D9" si="3">SUMPRODUCT(C2:C6,$E$2:$E$6)</f>
         <v>2.7490754138518101</v>
       </c>
-      <c r="E10" s="4">
+      <c r="D9" s="4">
         <f t="shared" si="3"/>
         <v>0.63594080698194932</v>
       </c>
-      <c r="F10" s="2"/>
-      <c r="G10" s="5"/>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="5"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B99C966B-08ED-4BF7-A8F0-824F4F9F7618}">
+  <dimension ref="A1:D10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="2"/>
+      <c r="B1" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="18">
+        <v>2569.6059570000002</v>
+      </c>
+      <c r="C2" s="26">
+        <v>8.6436410000000006</v>
+      </c>
+      <c r="D2" s="7">
+        <f>C2/B2</f>
+        <v>3.3638001875164552E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="19">
+        <v>2568.584961</v>
+      </c>
+      <c r="C3" s="8">
+        <v>8.3340200000000006</v>
+      </c>
+      <c r="D3" s="1">
+        <f t="shared" ref="D3:D10" si="0">C3/B3</f>
+        <v>3.2445958091864733E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="19">
+        <v>1881.5654300000001</v>
+      </c>
+      <c r="C4" s="8">
+        <v>8.6143239999999999</v>
+      </c>
+      <c r="D4" s="1">
+        <f t="shared" si="0"/>
+        <v>4.578275016457971E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="19">
+        <v>1087.135376</v>
+      </c>
+      <c r="C5" s="8">
+        <v>3.5266820000000001</v>
+      </c>
+      <c r="D5" s="1">
+        <f t="shared" si="0"/>
+        <v>3.2440136507893387E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="19">
+        <v>1.9473000000000001E-2</v>
+      </c>
+      <c r="C6" s="8">
+        <v>5.6849999999999999E-3</v>
+      </c>
+      <c r="D6" s="1">
+        <f t="shared" si="0"/>
+        <v>0.29194268987829303</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="19">
+        <v>-4.1975999999999999E-2</v>
+      </c>
+      <c r="C7" s="8">
+        <v>2.3181E-2</v>
+      </c>
+      <c r="D7" s="1">
+        <f t="shared" si="0"/>
+        <v>-0.55224413950829043</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="19">
+        <v>-2.7300000000000002E-4</v>
+      </c>
+      <c r="C8" s="8">
+        <v>4.5800000000000002E-4</v>
+      </c>
+      <c r="D8" s="1">
+        <f t="shared" si="0"/>
+        <v>-1.6776556776556777</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="19">
+        <v>-1.083E-3</v>
+      </c>
+      <c r="C9" s="8">
+        <v>9.7099999999999997E-4</v>
+      </c>
+      <c r="D9" s="1">
+        <f t="shared" si="0"/>
+        <v>-0.89658356417359186</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="20">
+        <v>3.0603000000000002E-2</v>
+      </c>
+      <c r="C10" s="9">
+        <v>2.7059E-2</v>
+      </c>
+      <c r="D10" s="6">
+        <f t="shared" si="0"/>
+        <v>0.88419436003006235</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>